<commit_message>
die schiss Diagramm nomal chöne neu mache mit Geradene -.-
</commit_message>
<xml_diff>
--- a/m4a_physikpraktikum_stroemungen.xlsx
+++ b/m4a_physikpraktikum_stroemungen.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>Messungen 4.1</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Geschwindigkeit^2 [m/s]^2</t>
+  </si>
+  <si>
+    <t>Fehlerschranke Zeit</t>
   </si>
 </sst>
 </file>
@@ -513,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,7 +607,7 @@
         <v>0.94999999999999984</v>
       </c>
       <c r="I4" s="4">
-        <v>0.87934903791483088</v>
+        <v>0.87934903791483099</v>
       </c>
       <c r="J4" s="4">
         <v>0.02</v>
@@ -1089,6 +1092,12 @@
       <c r="G39">
         <v>4</v>
       </c>
+      <c r="I39" t="s">
+        <v>34</v>
+      </c>
+      <c r="J39">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="8"/>
@@ -1115,6 +1124,12 @@
         <f t="shared" si="14"/>
         <v>16</v>
       </c>
+      <c r="I40" t="s">
+        <v>2</v>
+      </c>
+      <c r="J40">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="8"/>
@@ -1215,11 +1230,11 @@
         <v>1.4236226450908744E-2</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" ref="D45:G45" si="16">1/D44</f>
+        <f>1/D44</f>
         <v>3.3829499323410013E-2</v>
       </c>
       <c r="E45" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="D45:G45" si="16">1/E44</f>
         <v>5.3003533568904596E-2</v>
       </c>
       <c r="F45" s="1">
@@ -1227,7 +1242,7 @@
         <v>8.0299785867237683E-2</v>
       </c>
       <c r="G45" s="1">
-        <f t="shared" si="16"/>
+        <f>1/G44</f>
         <v>0.14866204162537167</v>
       </c>
     </row>

</xml_diff>